<commit_message>
began writing single image analysis function, lots of FIXME's
</commit_message>
<xml_diff>
--- a/CNNgraph.xlsx
+++ b/CNNgraph.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\Repo498\fractal-eyes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Diego/Documents/School/Senior Design/Fractal-Eyes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6CFE2B-8045-4B1C-85C3-6A16E6B8C1E4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8D6B74-AD83-514E-B24E-E04C720C3321}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9836349A-661D-435B-A434-6A2150466024}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{9836349A-661D-435B-A434-6A2150466024}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$11</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$2:$B$11</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -297,6 +302,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Epochs</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -359,6 +419,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Percent</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Accuracy</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1013,15 +1133,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>599440</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1349,16 +1469,15 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+    <col min="1" max="2" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1366,7 +1485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1374,7 +1493,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1382,7 +1501,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1390,7 +1509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1398,7 +1517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1406,7 +1525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1414,7 +1533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1422,7 +1541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1430,7 +1549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1438,7 +1557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>

</xml_diff>